<commit_message>
add more injury data
</commit_message>
<xml_diff>
--- a/data/phenotypes/Injury data.xlsx
+++ b/data/phenotypes/Injury data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vistor/Documents/Work/GitHub/PhD/ms_epi_effort/data/phenotypes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD62982-3C44-FE45-A046-182C138BC927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{249F0425-C15D-1647-ADC2-54AAFE5876C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="28800" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="91">
   <si>
     <t>Date</t>
   </si>
@@ -297,13 +297,52 @@
   </si>
   <si>
     <t>injury_belly</t>
+  </si>
+  <si>
+    <t>D229161</t>
+  </si>
+  <si>
+    <t>D229103</t>
+  </si>
+  <si>
+    <t>D229097</t>
+  </si>
+  <si>
+    <t>D229735</t>
+  </si>
+  <si>
+    <t>D229658</t>
+  </si>
+  <si>
+    <t>D229025</t>
+  </si>
+  <si>
+    <t>D229776</t>
+  </si>
+  <si>
+    <t>D237389</t>
+  </si>
+  <si>
+    <t>D229775</t>
+  </si>
+  <si>
+    <t>D237278</t>
+  </si>
+  <si>
+    <t>D237361</t>
+  </si>
+  <si>
+    <t>D237378</t>
+  </si>
+  <si>
+    <t>D229162</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,12 +356,6 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -357,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -365,6 +398,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,10 +750,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H77"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2723,6 +2757,490 @@
         <v>61</v>
       </c>
     </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="7">
+        <v>38485</v>
+      </c>
+      <c r="B78" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="7">
+        <v>38485</v>
+      </c>
+      <c r="B79" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="7">
+        <v>38843</v>
+      </c>
+      <c r="B80" t="s">
+        <v>79</v>
+      </c>
+      <c r="C80">
+        <v>1190</v>
+      </c>
+      <c r="D80">
+        <v>5</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>0.6</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="7">
+        <v>38844</v>
+      </c>
+      <c r="B81" t="s">
+        <v>80</v>
+      </c>
+      <c r="C81">
+        <v>1230</v>
+      </c>
+      <c r="D81">
+        <v>10</v>
+      </c>
+      <c r="E81">
+        <v>5</v>
+      </c>
+      <c r="F81">
+        <v>40</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="7">
+        <v>38847</v>
+      </c>
+      <c r="B82" t="s">
+        <v>9</v>
+      </c>
+      <c r="C82">
+        <v>1290</v>
+      </c>
+      <c r="D82">
+        <v>15</v>
+      </c>
+      <c r="E82">
+        <v>10</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>1</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="7">
+        <v>39206</v>
+      </c>
+      <c r="B83" t="s">
+        <v>11</v>
+      </c>
+      <c r="C83">
+        <v>1220</v>
+      </c>
+      <c r="D83">
+        <v>15</v>
+      </c>
+      <c r="E83">
+        <v>35</v>
+      </c>
+      <c r="F83">
+        <v>50</v>
+      </c>
+      <c r="G83">
+        <v>1.5</v>
+      </c>
+      <c r="H83">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="7">
+        <v>39207</v>
+      </c>
+      <c r="B84" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84">
+        <v>1250</v>
+      </c>
+      <c r="D84">
+        <v>15</v>
+      </c>
+      <c r="E84">
+        <v>15</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>3.6</v>
+      </c>
+      <c r="H84">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="7">
+        <v>39207</v>
+      </c>
+      <c r="B85" t="s">
+        <v>42</v>
+      </c>
+      <c r="C85">
+        <v>1260</v>
+      </c>
+      <c r="D85">
+        <v>20</v>
+      </c>
+      <c r="E85">
+        <v>15</v>
+      </c>
+      <c r="F85">
+        <v>5</v>
+      </c>
+      <c r="G85">
+        <v>2.5</v>
+      </c>
+      <c r="H85">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="7">
+        <v>39208</v>
+      </c>
+      <c r="B86" t="s">
+        <v>55</v>
+      </c>
+      <c r="C86">
+        <v>1350</v>
+      </c>
+      <c r="D86">
+        <v>30</v>
+      </c>
+      <c r="E86">
+        <v>10</v>
+      </c>
+      <c r="F86">
+        <v>5</v>
+      </c>
+      <c r="G86">
+        <v>0.8</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="7">
+        <v>39208</v>
+      </c>
+      <c r="B87" t="s">
+        <v>17</v>
+      </c>
+      <c r="C87">
+        <v>1310</v>
+      </c>
+      <c r="D87">
+        <v>15</v>
+      </c>
+      <c r="E87">
+        <v>10</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="7">
+        <v>39208</v>
+      </c>
+      <c r="B88" t="s">
+        <v>81</v>
+      </c>
+      <c r="C88">
+        <v>1330</v>
+      </c>
+      <c r="D88">
+        <v>15</v>
+      </c>
+      <c r="E88">
+        <v>10</v>
+      </c>
+      <c r="F88">
+        <v>5</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="7">
+        <v>39209</v>
+      </c>
+      <c r="B89" t="s">
+        <v>82</v>
+      </c>
+      <c r="C89">
+        <v>1180</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>0.3</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="7">
+        <v>39209</v>
+      </c>
+      <c r="B90" t="s">
+        <v>83</v>
+      </c>
+      <c r="C90">
+        <v>1170</v>
+      </c>
+      <c r="D90">
+        <v>10</v>
+      </c>
+      <c r="E90">
+        <v>5</v>
+      </c>
+      <c r="F90">
+        <v>5</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="7">
+        <v>39211</v>
+      </c>
+      <c r="B91" t="s">
+        <v>84</v>
+      </c>
+      <c r="C91">
+        <v>1190</v>
+      </c>
+      <c r="D91">
+        <v>25</v>
+      </c>
+      <c r="E91">
+        <v>20</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>8</v>
+      </c>
+      <c r="H91">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="7">
+        <v>39211</v>
+      </c>
+      <c r="B92" t="s">
+        <v>85</v>
+      </c>
+      <c r="C92">
+        <v>1200</v>
+      </c>
+      <c r="D92">
+        <v>10</v>
+      </c>
+      <c r="E92">
+        <v>20</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="7">
+        <v>39212</v>
+      </c>
+      <c r="B93" t="s">
+        <v>86</v>
+      </c>
+      <c r="C93">
+        <v>1200</v>
+      </c>
+      <c r="D93">
+        <v>30</v>
+      </c>
+      <c r="E93">
+        <v>30</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+      <c r="H93">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="7">
+        <v>39217</v>
+      </c>
+      <c r="B94" t="s">
+        <v>87</v>
+      </c>
+      <c r="C94">
+        <v>1210</v>
+      </c>
+      <c r="D94">
+        <v>15</v>
+      </c>
+      <c r="E94">
+        <v>20</v>
+      </c>
+      <c r="F94">
+        <v>60</v>
+      </c>
+      <c r="G94">
+        <v>0.9</v>
+      </c>
+      <c r="H94">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="7">
+        <v>39217</v>
+      </c>
+      <c r="B95" t="s">
+        <v>88</v>
+      </c>
+      <c r="C95">
+        <v>1100</v>
+      </c>
+      <c r="D95">
+        <v>5</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+      <c r="H95">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="7">
+        <v>39217</v>
+      </c>
+      <c r="B96" t="s">
+        <v>89</v>
+      </c>
+      <c r="C96">
+        <v>1160</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>5</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>1.2</v>
+      </c>
+      <c r="H96">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="7">
+        <v>39217</v>
+      </c>
+      <c r="B97" t="s">
+        <v>90</v>
+      </c>
+      <c r="C97">
+        <v>1220</v>
+      </c>
+      <c r="D97">
+        <v>25</v>
+      </c>
+      <c r="E97">
+        <v>15</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>7</v>
+      </c>
+      <c r="H97">
+        <v>2.4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>